<commit_message>
Tidsplan, skrivevejledning og roller
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Milepæle</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Tidspunkt</t>
   </si>
   <si>
-    <t>Problem analysen SKAL være færdig inden statusseminariet</t>
-  </si>
-  <si>
     <t>Programmeringen skal gerne være påbegyndt inden statusseminariet</t>
   </si>
   <si>
@@ -54,13 +51,40 @@
   </si>
   <si>
     <t>Rapporten skal afleveres torsdag d. 18/12 kl. 12.00</t>
+  </si>
+  <si>
+    <t>Interview</t>
+  </si>
+  <si>
+    <t>Sendes til Mona d. 20/10 kl. 12.00</t>
+  </si>
+  <si>
+    <t>Klaret/ikke klaret</t>
+  </si>
+  <si>
+    <t>Interview guide</t>
+  </si>
+  <si>
+    <t>Laver interview guide onsdag d. 15/10</t>
+  </si>
+  <si>
+    <t>Udførelse af interview</t>
+  </si>
+  <si>
+    <t>Så hurtigt som muligt, gerne inden d. 20/10</t>
+  </si>
+  <si>
+    <t>Problem analysen SKAL sendes til Mona 30/12 kl. 12</t>
+  </si>
+  <si>
+    <t>Hvornår blev det færdigt?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +115,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,11 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,11 +202,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D8" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Milepæle" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Tidspunkt"/>
+    <tableColumn id="3" name="Klaret/ikke klaret"/>
+    <tableColumn id="4" name="Hvornår blev det færdigt?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,56 +477,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.109375" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>